<commit_message>
[Pravek Saxena]: Added a line "Reviewed by Pravek" for demonstration purpose of working of SVN to Ram
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltAndBerylInternship_Repo\trunk\DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="9735"/>
   </bookViews>
@@ -24,7 +29,7 @@
     <author>Pravek Saxena</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
+    <comment ref="E13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0">
+    <comment ref="H13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0">
+    <comment ref="A22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="C22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>Batch</t>
   </si>
@@ -422,6 +427,9 @@
   </si>
   <si>
     <t>userName</t>
+  </si>
+  <si>
+    <t>Reviewed by Pravek</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1262,7 +1270,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,6 +1299,9 @@
         <v>2</v>
       </c>
       <c r="F1" s="5"/>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
Ruchi Pareek : Added new table "ShowInterest" in All Tables Sheet.xlsx
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltandBeryl\Margdarshak\Industry_Internship\Internship_2017_Prep.git\trunk\DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="All Tables" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -16,10 +24,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Ruchi Pareek</author>
     <author>Pravek Saxena</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added a new table Show Interest | 18-05-2017</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -33,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0">
+    <comment ref="G13" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="E14" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0">
+    <comment ref="A18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="C22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>Batch</t>
   </si>
@@ -438,13 +471,25 @@
   </si>
   <si>
     <t>Revised by Achin</t>
+  </si>
+  <si>
+    <t>Show Interest</t>
+  </si>
+  <si>
+    <t>BatchID</t>
+  </si>
+  <si>
+    <t>ShowInterest</t>
+  </si>
+  <si>
+    <t>Revised by Ruchi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,8 +577,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +727,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF97C1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,20 +1087,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF97C1"/>
+      <color rgb="FFFF0066"/>
       <color rgb="FFFF33CC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1291,7 +1400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1301,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,11 +1420,11 @@
     <col min="2" max="2" width="4.28515625" style="54" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="19" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -1330,7 +1439,7 @@
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="92" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1346,7 +1455,7 @@
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="92" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1361,6 +1470,9 @@
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
         <v>7</v>
+      </c>
+      <c r="I3" s="92" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1657,6 +1769,9 @@
       <c r="E22" s="55" t="s">
         <v>11</v>
       </c>
+      <c r="I22" s="90" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
@@ -1668,7 +1783,9 @@
     <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="51"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="27"/>
+      <c r="C24" s="89" t="s">
+        <v>115</v>
+      </c>
       <c r="E24" s="49" t="s">
         <v>24</v>
       </c>
@@ -1676,7 +1793,9 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
       <c r="B25" s="48"/>
-      <c r="C25" s="27"/>
+      <c r="C25" s="91" t="s">
+        <v>116</v>
+      </c>
       <c r="E25" s="50" t="s">
         <v>11</v>
       </c>
@@ -1684,6 +1803,9 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="17"/>
+      <c r="C26" s="91" t="s">
+        <v>32</v>
+      </c>
       <c r="E26" s="63" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Ruchi Pareek : All Tables Sheet.xlsx to add one new table
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -1410,13 +1410,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" style="54" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="19" customWidth="1"/>

</xml_diff>

<commit_message>
Author           : Ruchi Pareek Description      : Updated DB schema, added tables CSV Upload, Documents Uploaded and changed Application Table
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -121,12 +121,180 @@
         </r>
       </text>
     </comment>
+    <comment ref="G27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of document+username+timestamp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+File system location</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C32" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This field value can have duplicate value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Primary key, Auto increment, Integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C37" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Boolean with a value true for the latest row and false for previous rows</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+User does not exist</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Type of User</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="133">
   <si>
     <t>Batch</t>
   </si>
@@ -329,9 +497,6 @@
     <t>MobileTC</t>
   </si>
   <si>
-    <t>TP Application</t>
-  </si>
-  <si>
     <t>Application Id</t>
   </si>
   <si>
@@ -452,9 +617,6 @@
     <t>Pincode</t>
   </si>
   <si>
-    <t>TP Id</t>
-  </si>
-  <si>
     <t xml:space="preserve"> TP Application</t>
   </si>
   <si>
@@ -483,6 +645,54 @@
   </si>
   <si>
     <t>Revised by Ruchi</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>ACTIVE_FLAG</t>
+  </si>
+  <si>
+    <t>DocumentsUploaded</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>OriginalApplicationId</t>
+  </si>
+  <si>
+    <t>DocumentName</t>
+  </si>
+  <si>
+    <t>DocumentLocation</t>
+  </si>
+  <si>
+    <t>CSVUploaded</t>
+  </si>
+  <si>
+    <t>CSVId</t>
+  </si>
+  <si>
+    <t>DocumentId</t>
+  </si>
+  <si>
+    <t>CSVType</t>
+  </si>
+  <si>
+    <t>CSVName</t>
+  </si>
+  <si>
+    <t>CSVLocation</t>
+  </si>
+  <si>
+    <t>ApplicationID</t>
   </si>
 </sst>
 </file>
@@ -591,7 +801,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,6 +949,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF97C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1036,9 +1258,6 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1074,7 +1293,6 @@
     <xf numFmtId="0" fontId="9" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1093,6 +1311,16 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1410,19 +1638,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" style="54" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="19" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1439,8 +1667,8 @@
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="92" t="s">
-        <v>103</v>
+      <c r="I1" s="90" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1455,8 +1683,8 @@
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="92" t="s">
-        <v>114</v>
+      <c r="I2" s="90" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1464,15 +1692,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="79" t="s">
-        <v>88</v>
+      <c r="C3" s="78" t="s">
+        <v>87</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="92" t="s">
-        <v>118</v>
+      <c r="I3" s="90" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1496,8 +1724,8 @@
       <c r="C5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="78" t="s">
-        <v>78</v>
+      <c r="E5" s="77" t="s">
+        <v>77</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>13</v>
@@ -1526,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="67" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1539,7 +1767,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="26"/>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="65" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="28" t="s">
@@ -1555,7 +1783,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="68" t="s">
         <v>27</v>
       </c>
       <c r="I9" s="29" t="s">
@@ -1571,11 +1799,11 @@
         <v>31</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="87" t="s">
-        <v>99</v>
+      <c r="E10" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="85" t="s">
+        <v>98</v>
       </c>
       <c r="I10" s="30" t="s">
         <v>25</v>
@@ -1590,11 +1818,11 @@
         <v>34</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="72" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>28</v>
@@ -1610,7 +1838,7 @@
       </c>
       <c r="D12" s="10"/>
       <c r="G12" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I12" s="32" t="s">
         <v>23</v>
@@ -1629,7 +1857,7 @@
         <v>25</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I13" s="34" t="s">
         <v>29</v>
@@ -1692,7 +1920,7 @@
       <c r="E17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="84" t="s">
+      <c r="I17" s="82" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1706,8 +1934,8 @@
       <c r="E18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="80" t="s">
-        <v>98</v>
+      <c r="I18" s="79" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -1722,8 +1950,8 @@
       <c r="E19" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="83" t="s">
-        <v>109</v>
+      <c r="I19" s="81" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,8 +1966,8 @@
       <c r="E20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="I20" s="86" t="s">
-        <v>95</v>
+      <c r="I20" s="84" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1752,10 +1980,10 @@
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="88" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+      <c r="I21" s="86" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1769,8 +1997,8 @@
       <c r="E22" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="90" t="s">
-        <v>117</v>
+      <c r="I22" s="88" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1779,58 +2007,82 @@
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="27"/>
+      <c r="I23" s="95" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="51"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="89" t="s">
-        <v>115</v>
+      <c r="C24" s="87" t="s">
+        <v>113</v>
       </c>
       <c r="E24" s="49" t="s">
         <v>24</v>
+      </c>
+      <c r="G24" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="94" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
       <c r="B25" s="48"/>
-      <c r="C25" s="91" t="s">
-        <v>116</v>
+      <c r="C25" s="89" t="s">
+        <v>114</v>
       </c>
       <c r="E25" s="50" t="s">
         <v>11</v>
+      </c>
+      <c r="G25" s="92" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="91" t="s">
+      <c r="C26" s="89" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="63" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>56</v>
       </c>
       <c r="B27" s="19"/>
+      <c r="C27" s="89" t="s">
+        <v>120</v>
+      </c>
       <c r="E27" s="63" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="G27" s="70" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="19"/>
       <c r="E28" s="61" t="s">
         <v>58</v>
       </c>
+      <c r="G28" s="70" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="52"/>
       <c r="D29" s="52"/>
@@ -1840,7 +2092,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="19"/>
       <c r="E30" s="61" t="s">
@@ -1848,24 +2100,32 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="71" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="76" t="s">
-        <v>67</v>
+      <c r="A31" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="75" t="s">
+        <v>121</v>
       </c>
       <c r="E31" s="61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" s="65" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="71" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="72"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="74"/>
+      <c r="G31" s="93" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="66"/>
+      <c r="E32" s="73"/>
+      <c r="G32" s="96" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
@@ -1873,85 +2133,100 @@
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="61" t="s">
         <v>61</v>
       </c>
+      <c r="G33" s="96" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E34" s="61" t="s">
         <v>64</v>
+      </c>
+      <c r="G34" s="96" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="53"/>
-      <c r="C35" s="82" t="s">
-        <v>108</v>
+      <c r="C35" s="59" t="s">
+        <v>122</v>
       </c>
       <c r="E35" s="61" t="s">
         <v>65</v>
+      </c>
+      <c r="G35" s="96" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
+      <c r="C36" s="58" t="s">
+        <v>117</v>
+      </c>
       <c r="E36" s="61" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
+      <c r="C37" s="58" t="s">
+        <v>118</v>
+      </c>
       <c r="E37" s="61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B38" s="19"/>
       <c r="E38" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="81" t="s">
-        <v>105</v>
+        <v>71</v>
+      </c>
+      <c r="G38" s="80" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" s="19"/>
       <c r="E39" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E40" s="61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" s="58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E41" s="61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G41" s="58" t="s">
         <v>62</v>
@@ -1959,10 +2234,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G42" s="58" t="s">
         <v>63</v>
@@ -1970,10 +2245,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" s="58" t="s">
         <v>57</v>
@@ -1981,66 +2256,69 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="E44" s="63" t="s">
+        <v>132</v>
       </c>
       <c r="G44" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G45" s="58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G46" s="58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A49" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="62" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A49" s="85" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="85" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="66" t="s">
-        <v>112</v>
-      </c>
-      <c r="G50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="70" t="s">
+      <c r="C52" s="74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="74" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="75" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="75" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Author       :Shubham Jain Description  :For git session to understand resolving of conflicts
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltandBeryl\Margdarshak\Industry_Internship\Internship_2017_Prep.git\trunk\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017\trunk\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -294,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
   <si>
     <t>Batch</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>ApplicationID</t>
+  </si>
+  <si>
+    <t>Changed by Shubham</t>
   </si>
 </sst>
 </file>
@@ -965,7 +968,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1123,11 +1126,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1321,6 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1638,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,6 +1730,9 @@
       <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
+      <c r="I4" s="97" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">

</xml_diff>

<commit_message>
Author: Pravek Saxena Description : Modified and corrected the table as per the flow discussion with Ruchi and basis change in business requirements as per discussion with SCGJ people
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltandBeryl\Margdarshak\Industry_Internship\Internship_2017_Prep.git\trunk\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pravek Saxena\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,11 +24,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Pravek Saxena</author>
     <author>Ruchi Pareek</author>
-    <author>Pravek Saxena</author>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pravek Saxena:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This serves as the Draft table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,24 +84,23 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ruchi Pareek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pravek Saxena:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Name of Institution to be used as unique field
-</t>
+This is not the training partner ID as received from SDMS. It is just a primary key of the table</t>
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,13 +133,189 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Added from my side</t>
+            <charset val="1"/>
+          </rPr>
+          <t>Pravek Saxena:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Primary Key
+This is the email ID of the user</t>
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>There will be a checkbox field to capture this upfront
+TP
+AP
+SCGJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Added from my side</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pravek Saxena:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+temp
+registered</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Primary key, Auto increment, Integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Boolean with a value true for the latest row and false for previous rows</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Added from my side</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L17" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Name of document+username+timestamp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L18" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+File system location</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0" shapeId="0">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,23 +347,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ruchi Pareek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Primary key, Auto increment, Integer</t>
+            <family val="2"/>
+          </rPr>
+          <t>Added from my side</t>
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0">
+    <comment ref="N21" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +361,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Ruchi Pareek:</t>
         </r>
@@ -181,14 +370,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Boolean with a value true for the latest row and false for previous rows</t>
+User does not exist</t>
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="1" shapeId="0">
+    <comment ref="J23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,11 +387,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Added from my side</t>
+          <t>Pravek Saxena:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the userId </t>
         </r>
       </text>
     </comment>
-    <comment ref="L17" authorId="0" shapeId="0">
+    <comment ref="L24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,21 +411,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ruchi Pareek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Name of document+username+timestamp</t>
+          <t>Added from my side</t>
         </r>
       </text>
     </comment>
-    <comment ref="L18" authorId="0" shapeId="0">
+    <comment ref="A26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -236,21 +425,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ruchi Pareek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-File system location</t>
+          <t>Added from my side</t>
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="1" shapeId="0">
+    <comment ref="H26" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,65 +437,23 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Added from my side</t>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This field value can have duplicate value</t>
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Added from my side</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C27" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Added from my side</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Ruchi Pareek:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-User does not exist</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H33" authorId="1" shapeId="0">
+    <comment ref="C27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +472,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
   <si>
     <t>Batch</t>
   </si>
@@ -373,9 +510,6 @@
     <t xml:space="preserve">District </t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>FaxNumber</t>
   </si>
   <si>
@@ -403,51 +537,27 @@
     <t>MobileTC</t>
   </si>
   <si>
-    <t>TP ID</t>
-  </si>
-  <si>
     <t>Turnover -Format- Cr-Lakhs</t>
   </si>
   <si>
-    <t>AddressID</t>
-  </si>
-  <si>
-    <t>Line2</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
-    <t>Line 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address ID </t>
-  </si>
-  <si>
     <t>TPManagement</t>
   </si>
   <si>
     <t>TPManagementID</t>
   </si>
   <si>
-    <t>Designation | Format  - Director || Operation head etc</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>ContactInfoId</t>
-  </si>
-  <si>
     <t>EmailId</t>
   </si>
   <si>
-    <t>ContactInfoID</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
@@ -463,15 +573,9 @@
     <t>User</t>
   </si>
   <si>
-    <t>username - emailId</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>ContactInfo</t>
-  </si>
-  <si>
     <t>BusinessAudit</t>
   </si>
   <si>
@@ -481,33 +585,15 @@
     <t>AuditMessage</t>
   </si>
   <si>
-    <t>userName</t>
-  </si>
-  <si>
     <t>Reviewed by Pravek</t>
   </si>
   <si>
-    <t>ContactInfomation</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
     <t>Pincode</t>
   </si>
   <si>
-    <t>Authority</t>
-  </si>
-  <si>
-    <t>authType</t>
-  </si>
-  <si>
-    <t>authorityId</t>
-  </si>
-  <si>
-    <t>AuthorityId</t>
-  </si>
-  <si>
     <t>Revised by Achin</t>
   </si>
   <si>
@@ -517,9 +603,6 @@
     <t>BatchID</t>
   </si>
   <si>
-    <t>ShowInterest</t>
-  </si>
-  <si>
     <t>Revised by Ruchi</t>
   </si>
   <si>
@@ -535,9 +618,6 @@
     <t>Application</t>
   </si>
   <si>
-    <t>OriginalApplicationId</t>
-  </si>
-  <si>
     <t>DocumentName</t>
   </si>
   <si>
@@ -574,42 +654,18 @@
     <t>trainingPartnerName</t>
   </si>
   <si>
-    <t>trainingPartnerID</t>
-  </si>
-  <si>
-    <t>originalApplicationId</t>
-  </si>
-  <si>
     <t>application Id</t>
   </si>
   <si>
-    <t>application Status</t>
-  </si>
-  <si>
     <t>userId</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
     <t>Tables to store data generated from our system</t>
   </si>
   <si>
-    <t>AssessmentAgencyRegistartion</t>
-  </si>
-  <si>
-    <t>SaveAsDraftTrainingPartner</t>
-  </si>
-  <si>
-    <t>agencySSDMSID</t>
-  </si>
-  <si>
     <t>isNSDCfunded - bool</t>
   </si>
   <si>
-    <t>ApplicationID - FK</t>
-  </si>
-  <si>
     <t>YearOfRecoginition - YYYY</t>
   </si>
   <si>
@@ -631,9 +687,6 @@
     <t>Year of Establisment - YYYY</t>
   </si>
   <si>
-    <t>tpManagmentID - FK</t>
-  </si>
-  <si>
     <t>website - varchar</t>
   </si>
   <si>
@@ -784,9 +837,6 @@
     <t>Training Partner Name - varchar2</t>
   </si>
   <si>
-    <t>originalApplicationId - FK</t>
-  </si>
-  <si>
     <t>Centre ID -int</t>
   </si>
   <si>
@@ -841,20 +891,77 @@
     <t>Location Of Employer State - varchar2</t>
   </si>
   <si>
-    <t>originalapplicationId</t>
-  </si>
-  <si>
-    <t>all fields of TrainingPartnerRegistration</t>
-  </si>
-  <si>
-    <t>All the fields of AssessmentAgencyRegistration</t>
+    <t>BatchMode - varchar2</t>
+  </si>
+  <si>
+    <t>AssessmentAgencyRegistration</t>
+  </si>
+  <si>
+    <t>user_role</t>
+  </si>
+  <si>
+    <t>sPOC_Name</t>
+  </si>
+  <si>
+    <t>organization_Name</t>
+  </si>
+  <si>
+    <t>user_status</t>
+  </si>
+  <si>
+    <t>application State</t>
+  </si>
+  <si>
+    <t>CSV_Upload_Date</t>
+  </si>
+  <si>
+    <t>CSV_Upload_UserId - FK</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Application Comments</t>
+  </si>
+  <si>
+    <t>CommentID</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>applicationId -FK</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Batches Accepted</t>
+  </si>
+  <si>
+    <t>application Id - FK</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>TpID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designation </t>
+  </si>
+  <si>
+    <t>ABId</t>
+  </si>
+  <si>
+    <t>Fields to be added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -962,8 +1069,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,12 +1218,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF97C1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1120,20 +1228,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1297,17 +1393,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -1319,7 +1404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1362,7 +1447,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1380,8 +1464,6 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1400,13 +1482,7 @@
     <xf numFmtId="0" fontId="5" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1415,24 +1491,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1477,30 +1549,44 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1816,439 +1902,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" style="7" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="52" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="12" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="65" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:12" s="58" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="H1" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="81"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="H1" s="89" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-    </row>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="82" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="B5" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="61" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" s="85" t="s">
-        <v>169</v>
-      </c>
-      <c r="O3" s="83" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="86" t="s">
-        <v>168</v>
-      </c>
-      <c r="O4" s="84" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="I5" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="76" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="68" t="s">
-        <v>129</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="H6" s="51"/>
+      <c r="I6" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="83" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="I7" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="77" t="s">
+      <c r="C10" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="80" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="67" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="I8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="74" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="I9" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L9" s="57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="C12" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" s="79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="69" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="I10" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="D13" s="4"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="I11" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="L11" s="57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="74" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="I12" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="C14" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="69" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="I13" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="I14" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="I15" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="60" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>157</v>
+      <c r="C16" s="67" t="s">
+        <v>128</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="36"/>
-      <c r="L16" s="44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="74" t="s">
-        <v>158</v>
+        <v>57</v>
+      </c>
+      <c r="H16" s="51"/>
+      <c r="I16" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>129</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="36"/>
-      <c r="L17" s="41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>104</v>
+      <c r="H17" s="51"/>
+      <c r="I17" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="36"/>
-      <c r="L18" s="41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>142</v>
+      <c r="H18" s="51"/>
+      <c r="I18" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>114</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19" s="36"/>
-    </row>
-    <row r="20" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="75" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="69" t="s">
-        <v>143</v>
+      <c r="H19" s="51"/>
+      <c r="I19" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>115</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>7</v>
@@ -2256,337 +2357,335 @@
       <c r="E20" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="36"/>
-    </row>
-    <row r="21" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="75" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="69" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>159</v>
+      <c r="H20" s="51"/>
+      <c r="I20" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>130</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="36"/>
-      <c r="L21" s="61" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="75" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="75" t="s">
-        <v>160</v>
+        <v>23</v>
+      </c>
+      <c r="I21" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="87"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>131</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" s="64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="76" t="s">
-        <v>149</v>
+      <c r="L22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>155</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="L23" s="64" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="L24" s="64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="78" t="s">
-        <v>123</v>
+      <c r="H24" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="L24" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" s="35"/>
+    </row>
+    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="71" t="s">
+        <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J25" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="90" t="s">
+        <v>154</v>
+      </c>
+      <c r="N25" s="35"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="91" t="s">
+        <v>153</v>
+      </c>
+      <c r="L26" s="33"/>
+      <c r="N26" s="35"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="92" t="s">
+        <v>42</v>
+      </c>
+      <c r="N27" s="35"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="N28" s="35"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="H29" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="N29" s="35"/>
+    </row>
+    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="H30" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="H31" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="33"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="64" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="79" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" s="36"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H28" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="24" t="s">
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="D33" s="35"/>
+      <c r="H33" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="36"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="J29" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="36"/>
-    </row>
-    <row r="30" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="92" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="H30" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" s="41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="H31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H32" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="J32" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" s="48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B33" s="42"/>
-      <c r="D33" s="38"/>
-      <c r="H33" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="J33" s="11"/>
+      <c r="L33"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="J34" s="36"/>
-      <c r="L34" s="31" t="s">
-        <v>35</v>
-      </c>
+      <c r="H34" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="B35" s="7"/>
-      <c r="J35" s="36"/>
-      <c r="L35" s="31" t="s">
-        <v>17</v>
-      </c>
+      <c r="H35" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="28"/>
-      <c r="J36" s="36"/>
-      <c r="L36" s="31" t="s">
-        <v>18</v>
-      </c>
+      <c r="B36" s="27"/>
+      <c r="H36" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
-      <c r="J37" s="36"/>
-      <c r="L37" s="31" t="s">
-        <v>13</v>
-      </c>
+      <c r="H37" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="45"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
-      <c r="J38" s="36"/>
-      <c r="L38" s="31" t="s">
-        <v>32</v>
-      </c>
+      <c r="H38" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
-      <c r="J39" s="11"/>
-      <c r="L39" s="31" t="s">
-        <v>37</v>
-      </c>
+      <c r="J39" s="44"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
-      <c r="J40" s="36"/>
-      <c r="L40" s="31" t="s">
-        <v>33</v>
-      </c>
+      <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J41" s="36"/>
+      <c r="J41" s="48"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J42" s="36"/>
+      <c r="J42" s="50"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J43" s="50" t="s">
-        <v>12</v>
-      </c>
+      <c r="J43" s="56"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J44" s="47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J45" s="49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J46" s="52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J47" s="54" t="s">
-        <v>45</v>
-      </c>
+      <c r="J44" s="55"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J48" s="56" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="J49" s="63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="J50" s="62" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I54" s="8" t="s">
+      <c r="I48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I55" s="9" t="s">
+    <row r="52" spans="9:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I52" s="9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Author: Pravek Saxena Description :  Removed the field Date of Joining from candidate table and added in the Employer table. @Ruchit Jain will make the suitable change in the excel import functionality
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pravek Saxena\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltAndBerylInternship_Repo\trunk\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -804,9 +804,6 @@
     <t>Trainee PIN Code - int</t>
   </si>
   <si>
-    <t>Result - bool</t>
-  </si>
-  <si>
     <t>Marks Obtained-Practical - decimal</t>
   </si>
   <si>
@@ -955,6 +952,9 @@
   </si>
   <si>
     <t>Fields to be added</t>
+  </si>
+  <si>
+    <t>Result - varchar2</t>
   </si>
 </sst>
 </file>
@@ -1553,20 +1553,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1587,6 +1575,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1905,7 +1905,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,20 +1928,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="58" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
-      <c r="H1" s="76" t="s">
+      <c r="H1" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="81"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91"/>
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="74" t="s">
@@ -1958,7 +1958,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>58</v>
@@ -1978,23 +1978,23 @@
         <v>98</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="51" t="s">
         <v>40</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="L3" s="79" t="s">
-        <v>153</v>
+        <v>142</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2005,22 +2005,22 @@
         <v>99</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="51" t="s">
         <v>43</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="L4" s="82" t="s">
+        <v>141</v>
+      </c>
+      <c r="L4" s="78" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="5"/>
       <c r="H5" s="51"/>
@@ -2042,7 +2042,7 @@
       <c r="J5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="78" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       <c r="J6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="83" t="s">
+      <c r="L6" s="79" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2075,7 +2075,7 @@
         <v>102</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="4"/>
       <c r="H7" s="51"/>
@@ -2083,7 +2083,7 @@
         <v>14</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -2094,18 +2094,18 @@
         <v>103</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="5"/>
       <c r="H8" s="51"/>
       <c r="I8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="79" t="s">
-        <v>144</v>
+      <c r="J8" s="76" t="s">
+        <v>143</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
         <v>104</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="10"/>
       <c r="H9" s="51"/>
@@ -2124,7 +2124,7 @@
         <v>15</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -2135,7 +2135,7 @@
         <v>105</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="4"/>
       <c r="H10" s="51"/>
@@ -2146,7 +2146,7 @@
         <v>47</v>
       </c>
       <c r="L10" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>107</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="4"/>
       <c r="H11" s="51"/>
@@ -2167,8 +2167,8 @@
       <c r="J11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="80" t="s">
-        <v>152</v>
+      <c r="L11" s="77" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>106</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D12" s="4"/>
       <c r="H12" s="51"/>
@@ -2187,9 +2187,9 @@
         <v>20</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="L12" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12" s="76" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2236,10 +2236,10 @@
         <v>85</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="4"/>
       <c r="H15" s="51"/>
@@ -2247,7 +2247,7 @@
         <v>21</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L15" s="53" t="s">
         <v>52</v>
@@ -2258,10 +2258,10 @@
         <v>86</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
@@ -2280,17 +2280,17 @@
         <v>87</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="51"/>
-      <c r="I17" s="84" t="s">
+      <c r="I17" s="80" t="s">
         <v>66</v>
       </c>
       <c r="J17" s="54" t="s">
@@ -2305,7 +2305,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>76</v>
@@ -2315,7 +2315,7 @@
         <v>7</v>
       </c>
       <c r="H18" s="51"/>
-      <c r="I18" s="84" t="s">
+      <c r="I18" s="80" t="s">
         <v>64</v>
       </c>
       <c r="J18" s="57" t="s">
@@ -2330,14 +2330,14 @@
         <v>89</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="51"/>
-      <c r="I19" s="84" t="s">
+      <c r="I19" s="80" t="s">
         <v>65</v>
       </c>
       <c r="J19" s="57" t="s">
@@ -2358,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="51"/>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="81" t="s">
         <v>60</v>
       </c>
       <c r="J20" s="57" t="s">
@@ -2369,11 +2369,11 @@
       <c r="A21" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="64" t="s">
         <v>116</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>9</v>
@@ -2381,26 +2381,26 @@
       <c r="H21" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="84" t="s">
+      <c r="I21" s="80" t="s">
         <v>63</v>
       </c>
       <c r="J21" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="88" t="s">
+      <c r="L21" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="N21" s="87"/>
+      <c r="N21" s="83"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="65" t="s">
         <v>117</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>1</v>
@@ -2408,11 +2408,11 @@
       <c r="H22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="84" t="s">
+      <c r="I22" s="80" t="s">
         <v>72</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>35</v>
@@ -2423,23 +2423,20 @@
       <c r="A23" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="65" t="s">
-        <v>118</v>
-      </c>
       <c r="C23" s="69" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I23" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="J23" s="89" t="s">
-        <v>147</v>
+      <c r="J23" s="85" t="s">
+        <v>146</v>
       </c>
       <c r="L23" s="30" t="s">
         <v>36</v>
@@ -2460,7 +2457,7 @@
         <v>29</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L24" s="31" t="s">
         <v>61</v>
@@ -2472,7 +2469,7 @@
         <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H25" s="23" t="s">
         <v>30</v>
@@ -2480,8 +2477,8 @@
       <c r="I25" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="90" t="s">
-        <v>154</v>
+      <c r="J25" s="86" t="s">
+        <v>153</v>
       </c>
       <c r="N25" s="35"/>
     </row>
@@ -2490,7 +2487,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H26" s="41" t="s">
         <v>60</v>
@@ -2498,8 +2495,8 @@
       <c r="I26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="91" t="s">
-        <v>153</v>
+      <c r="J26" s="87" t="s">
+        <v>152</v>
       </c>
       <c r="L26" s="33"/>
       <c r="N26" s="35"/>
@@ -2511,41 +2508,42 @@
       <c r="C27" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="H27" s="86" t="s">
-        <v>156</v>
+      <c r="H27" s="82" t="s">
+        <v>155</v>
       </c>
       <c r="I27" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="92" t="s">
+      <c r="J27" s="88" t="s">
         <v>42</v>
       </c>
       <c r="N27" s="35"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="71" t="s">
-        <v>139</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B28" s="7"/>
       <c r="H28" s="38" t="s">
         <v>38</v>
       </c>
       <c r="I28" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="92" t="s">
+      <c r="J28" s="88" t="s">
         <v>10</v>
       </c>
       <c r="N28" s="35"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
+      <c r="B29" s="35"/>
       <c r="H29" s="38" t="s">
         <v>39</v>
       </c>
       <c r="I29" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="93" t="s">
+      <c r="J29" s="89" t="s">
         <v>46</v>
       </c>
       <c r="N29" s="35"/>
@@ -2554,7 +2552,7 @@
       <c r="A30" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="7"/>
       <c r="D30" s="35"/>
       <c r="H30" s="37" t="s">
         <v>11</v>
@@ -2566,9 +2564,8 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="7"/>
+        <v>133</v>
+      </c>
       <c r="H31" s="37" t="s">
         <v>22</v>
       </c>
@@ -2579,8 +2576,9 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>135</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B32" s="39"/>
       <c r="H32" s="38" t="s">
         <v>27</v>
       </c>
@@ -2591,9 +2589,9 @@
     </row>
     <row r="33" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" s="39"/>
+        <v>135</v>
+      </c>
+      <c r="B33" s="7"/>
       <c r="D33" s="35"/>
       <c r="H33" s="38" t="s">
         <v>16</v>
@@ -2606,7 +2604,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="7"/>
       <c r="H34" s="38" t="s">
@@ -2619,9 +2617,9 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="B35" s="27"/>
       <c r="H35" s="38" t="s">
         <v>12</v>
       </c>
@@ -2631,8 +2629,10 @@
       <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="7"/>
       <c r="H36" s="38" t="s">
         <v>25</v>
       </c>
@@ -2658,7 +2658,6 @@
       <c r="J39" s="44"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
       <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author         : Priyanshu Pandey Task           : Files Modified Files Modified : All Tables Sheet.xlsx Description    : Excel Sheet For Tables is edited. A new field is added to the table 'Batch Assignment'
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmaltAndBerylInternship_Repo\trunk\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyanshu pandey\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,6 +26,7 @@
   <authors>
     <author>Pravek Saxena</author>
     <author>Ruchi Pareek</author>
+    <author>Priyanshu pandey</author>
   </authors>
   <commentList>
     <comment ref="I2" authorId="0" shapeId="0">
@@ -125,6 +126,117 @@
         </r>
       </text>
     </comment>
+    <comment ref="E5" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Priyanshu pandey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1. Renamed </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Batch Status </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">table to </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Batches Assignment
+2. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Added </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ResponseType</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> field to </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Batch Assignment Table </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">In </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tables to store data generated from our system</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -415,6 +527,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="J25" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="8"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Priyanshu pandey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="8"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Renamed the Table to Batch Assignment</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A26" authorId="0" shapeId="0">
       <text>
         <r>
@@ -464,6 +600,34 @@
             <family val="2"/>
           </rPr>
           <t>Added from my side</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J30" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Priyanshu pandey: This field stores the Assign Status of Assessment body</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Can have values:
+1. Proposed
+2. Accepted
+3. Rejected
+4. Not Acknowledged</t>
         </r>
       </text>
     </comment>
@@ -472,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="163">
   <si>
     <t>Batch</t>
   </si>
@@ -804,6 +968,9 @@
     <t>Trainee PIN Code - int</t>
   </si>
   <si>
+    <t>Result - bool</t>
+  </si>
+  <si>
     <t>Marks Obtained-Practical - decimal</t>
   </si>
   <si>
@@ -933,9 +1100,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Batches Accepted</t>
-  </si>
-  <si>
     <t>application Id - FK</t>
   </si>
   <si>
@@ -954,14 +1118,20 @@
     <t>Fields to be added</t>
   </si>
   <si>
-    <t>Result - varchar2</t>
+    <t>Revised by Priyanshu</t>
+  </si>
+  <si>
+    <t>ResponseType</t>
+  </si>
+  <si>
+    <t>Batch Assignment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1075,6 +1245,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="26">
@@ -1904,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,7 +2141,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>58</v>
@@ -1978,7 +2161,7 @@
         <v>98</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="51" t="s">
@@ -1991,10 +2174,10 @@
         <v>156</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L3" s="76" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2005,7 +2188,7 @@
         <v>99</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="51" t="s">
@@ -2018,7 +2201,7 @@
         <v>59</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L4" s="78" t="s">
         <v>42</v>
@@ -2035,6 +2218,9 @@
         <v>154</v>
       </c>
       <c r="D5" s="5"/>
+      <c r="E5" s="51" t="s">
+        <v>160</v>
+      </c>
       <c r="H5" s="51"/>
       <c r="I5" s="32" t="s">
         <v>70</v>
@@ -2075,7 +2261,7 @@
         <v>102</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4"/>
       <c r="H7" s="51"/>
@@ -2083,7 +2269,7 @@
         <v>14</v>
       </c>
       <c r="J7" s="51" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -2094,7 +2280,7 @@
         <v>103</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D8" s="5"/>
       <c r="H8" s="51"/>
@@ -2102,10 +2288,10 @@
         <v>15</v>
       </c>
       <c r="J8" s="76" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2116,7 +2302,7 @@
         <v>104</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D9" s="10"/>
       <c r="H9" s="51"/>
@@ -2124,7 +2310,7 @@
         <v>15</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
@@ -2135,7 +2321,7 @@
         <v>105</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D10" s="4"/>
       <c r="H10" s="51"/>
@@ -2146,7 +2332,7 @@
         <v>47</v>
       </c>
       <c r="L10" s="51" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2157,7 +2343,7 @@
         <v>107</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D11" s="4"/>
       <c r="H11" s="51"/>
@@ -2168,7 +2354,7 @@
         <v>60</v>
       </c>
       <c r="L11" s="77" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2179,7 +2365,7 @@
         <v>106</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D12" s="4"/>
       <c r="H12" s="51"/>
@@ -2187,7 +2373,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L12" s="76" t="s">
         <v>44</v>
@@ -2236,10 +2422,10 @@
         <v>85</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D15" s="4"/>
       <c r="H15" s="51"/>
@@ -2247,7 +2433,7 @@
         <v>21</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L15" s="53" t="s">
         <v>52</v>
@@ -2258,10 +2444,10 @@
         <v>86</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
@@ -2280,10 +2466,10 @@
         <v>87</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="13" t="s">
@@ -2305,7 +2491,7 @@
         <v>88</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>76</v>
@@ -2330,7 +2516,7 @@
         <v>89</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="15" t="s">
@@ -2369,11 +2555,11 @@
       <c r="A21" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="62" t="s">
         <v>116</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>9</v>
@@ -2396,11 +2582,11 @@
       <c r="A22" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="64" t="s">
         <v>117</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>1</v>
@@ -2412,7 +2598,7 @@
         <v>72</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>35</v>
@@ -2423,6 +2609,9 @@
       <c r="A23" s="68" t="s">
         <v>93</v>
       </c>
+      <c r="B23" s="65" t="s">
+        <v>118</v>
+      </c>
       <c r="C23" s="69" t="s">
         <v>154</v>
       </c>
@@ -2436,7 +2625,7 @@
         <v>71</v>
       </c>
       <c r="J23" s="85" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L23" s="30" t="s">
         <v>36</v>
@@ -2469,7 +2658,7 @@
         <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H25" s="23" t="s">
         <v>30</v>
@@ -2478,7 +2667,7 @@
         <v>38</v>
       </c>
       <c r="J25" s="86" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="N25" s="35"/>
     </row>
@@ -2487,7 +2676,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H26" s="41" t="s">
         <v>60</v>
@@ -2496,7 +2685,7 @@
         <v>39</v>
       </c>
       <c r="J26" s="87" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L26" s="33"/>
       <c r="N26" s="35"/>
@@ -2521,9 +2710,8 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="7"/>
+        <v>139</v>
+      </c>
       <c r="H28" s="38" t="s">
         <v>38</v>
       </c>
@@ -2536,7 +2724,7 @@
       <c r="N28" s="35"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
+      <c r="B29" s="7"/>
       <c r="H29" s="38" t="s">
         <v>39</v>
       </c>
@@ -2552,7 +2740,7 @@
       <c r="A30" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="35"/>
       <c r="D30" s="35"/>
       <c r="H30" s="37" t="s">
         <v>11</v>
@@ -2560,12 +2748,15 @@
       <c r="I30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="33"/>
+      <c r="J30" s="51" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>133</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B31" s="7"/>
       <c r="H31" s="37" t="s">
         <v>22</v>
       </c>
@@ -2576,9 +2767,8 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="39"/>
+        <v>135</v>
+      </c>
       <c r="H32" s="38" t="s">
         <v>27</v>
       </c>
@@ -2589,9 +2779,9 @@
     </row>
     <row r="33" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="B33" s="39"/>
       <c r="D33" s="35"/>
       <c r="H33" s="38" t="s">
         <v>16</v>
@@ -2604,7 +2794,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B34" s="7"/>
       <c r="H34" s="38" t="s">
@@ -2617,9 +2807,9 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="27"/>
+        <v>138</v>
+      </c>
+      <c r="B35" s="7"/>
       <c r="H35" s="38" t="s">
         <v>12</v>
       </c>
@@ -2629,10 +2819,8 @@
       <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="7"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="27"/>
       <c r="H36" s="38" t="s">
         <v>25</v>
       </c>
@@ -2658,6 +2846,7 @@
       <c r="J39" s="44"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
       <c r="J40" s="47"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author : Pushkar shukla Comment : All Tables Sheet revised by Pushkar.
</commit_message>
<xml_diff>
--- a/DB/All Tables Sheet.xlsx
+++ b/DB/All Tables Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyanshu pandey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSDMS-v1\trunk\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,6 +101,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="J3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Primary key</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E4" authorId="1" shapeId="0">
       <text>
         <r>
@@ -123,6 +147,30 @@
           <t xml:space="preserve">
 Updated 19-06-2016
 seperated tables csv imported and system generated</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ruchi Pareek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+unique key</t>
         </r>
       </text>
     </comment>
@@ -237,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,12 +305,26 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Primary Key
+Unique Key,
 This is the email ID of the user</t>
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Added from my side</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,21 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Added from my side</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J8" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -636,7 +684,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="165">
   <si>
     <t>Batch</t>
   </si>
@@ -857,9 +905,6 @@
     <t>e-mailDirector - varchar</t>
   </si>
   <si>
-    <t>Batches ID - int</t>
-  </si>
-  <si>
     <t>Batch Name - varchar2</t>
   </si>
   <si>
@@ -887,9 +932,6 @@
     <t>Job Role -varchar2</t>
   </si>
   <si>
-    <t>Job Role Code  - int</t>
-  </si>
-  <si>
     <t>Maximum Marks-Theory - decimal</t>
   </si>
   <si>
@@ -899,12 +941,6 @@
     <t>Level -varchar2</t>
   </si>
   <si>
-    <t>Result approved - bool</t>
-  </si>
-  <si>
-    <t>Result approved on date - bool</t>
-  </si>
-  <si>
     <t>Total Pass - int</t>
   </si>
   <si>
@@ -914,12 +950,6 @@
     <t>Total Not Appeared - int</t>
   </si>
   <si>
-    <t>Total Certify - int</t>
-  </si>
-  <si>
-    <t>Certificate downloaded - bool</t>
-  </si>
-  <si>
     <t>Batch assignment date - date</t>
   </si>
   <si>
@@ -938,12 +968,6 @@
     <t>Candidate Name  - varchar2</t>
   </si>
   <si>
-    <t>Enrollment Number - int</t>
-  </si>
-  <si>
-    <t>Gender - bool</t>
-  </si>
-  <si>
     <t>Date Of Birth - date</t>
   </si>
   <si>
@@ -968,21 +992,12 @@
     <t>Trainee PIN Code - int</t>
   </si>
   <si>
-    <t>Result - bool</t>
-  </si>
-  <si>
     <t>Marks Obtained-Practical - decimal</t>
   </si>
   <si>
     <t>Marks Obtained-Theory - decimal</t>
   </si>
   <si>
-    <t>Certified - bool</t>
-  </si>
-  <si>
-    <t>Placement Status - bool</t>
-  </si>
-  <si>
     <t>Date of joining - date</t>
   </si>
   <si>
@@ -1125,6 +1140,45 @@
   </si>
   <si>
     <t>Batch Assignment</t>
+  </si>
+  <si>
+    <t>id  int</t>
+  </si>
+  <si>
+    <t>Result approved - varchar</t>
+  </si>
+  <si>
+    <t>Result approved on date - date</t>
+  </si>
+  <si>
+    <t>Certificate downloaded - varchar</t>
+  </si>
+  <si>
+    <t>Revised by Pushkar</t>
+  </si>
+  <si>
+    <t>Job Role Code  - varchar</t>
+  </si>
+  <si>
+    <t>Total Certified - int</t>
+  </si>
+  <si>
+    <t>Batch ID - int</t>
+  </si>
+  <si>
+    <t>Enrollment Number - varchar</t>
+  </si>
+  <si>
+    <t>Gender - varchar</t>
+  </si>
+  <si>
+    <t>Result - varchar</t>
+  </si>
+  <si>
+    <t>Certified - varchar</t>
+  </si>
+  <si>
+    <t>Placement Status -varchar</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1314,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1411,6 +1465,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -1587,7 +1647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1758,6 +1818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2087,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,20 +2172,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="58" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92"/>
     </row>
     <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="74" t="s">
@@ -2141,7 +2202,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>58</v>
@@ -2155,53 +2216,53 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="51" t="s">
         <v>40</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="51" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="J3" s="90" t="s">
+        <v>152</v>
       </c>
       <c r="L3" s="76" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="51" t="s">
         <v>43</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L4" s="78" t="s">
         <v>42</v>
@@ -2209,24 +2270,24 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="51" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H5" s="51"/>
       <c r="I5" s="32" t="s">
         <v>70</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="L5" s="78" t="s">
         <v>10</v>
@@ -2234,20 +2295,23 @@
     </row>
     <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>8</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>156</v>
       </c>
       <c r="H6" s="51"/>
       <c r="I6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="37" t="s">
-        <v>33</v>
+      <c r="J6" s="51" t="s">
+        <v>61</v>
       </c>
       <c r="L6" s="79" t="s">
         <v>46</v>
@@ -2255,73 +2319,76 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D7" s="4"/>
       <c r="H7" s="51"/>
       <c r="I7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="51" t="s">
-        <v>141</v>
+      <c r="J7" s="37" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D8" s="5"/>
       <c r="H8" s="51"/>
       <c r="I8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="76" t="s">
-        <v>144</v>
+      <c r="J8" s="51" t="s">
+        <v>130</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D9" s="10"/>
       <c r="H9" s="51"/>
       <c r="I9" s="32" t="s">
         <v>15</v>
       </c>
+      <c r="J9" s="76" t="s">
+        <v>133</v>
+      </c>
       <c r="L9" s="34" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D10" s="4"/>
       <c r="H10" s="51"/>
@@ -2332,18 +2399,18 @@
         <v>47</v>
       </c>
       <c r="L10" s="51" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D11" s="4"/>
       <c r="H11" s="51"/>
@@ -2354,18 +2421,18 @@
         <v>60</v>
       </c>
       <c r="L11" s="77" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D12" s="4"/>
       <c r="H12" s="51"/>
@@ -2373,7 +2440,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="L12" s="76" t="s">
         <v>44</v>
@@ -2381,10 +2448,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D13" s="4"/>
       <c r="H13" s="51"/>
@@ -2397,10 +2464,10 @@
     </row>
     <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C14" s="36" t="s">
         <v>5</v>
@@ -2419,13 +2486,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D15" s="4"/>
       <c r="H15" s="51"/>
@@ -2433,7 +2500,7 @@
         <v>21</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="L15" s="53" t="s">
         <v>52</v>
@@ -2441,13 +2508,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="12" t="s">
@@ -2463,13 +2530,13 @@
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="68" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="13" t="s">
@@ -2488,13 +2555,13 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="14" t="s">
@@ -2513,10 +2580,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="68" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="15" t="s">
@@ -2532,10 +2599,10 @@
     </row>
     <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="68" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>7</v>
@@ -2553,13 +2620,13 @@
     </row>
     <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="68" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>9</v>
@@ -2580,13 +2647,13 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="68" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="B22" s="64" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>1</v>
@@ -2598,7 +2665,7 @@
         <v>72</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>35</v>
@@ -2607,25 +2674,25 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="68" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="I23" s="40" t="s">
         <v>71</v>
       </c>
       <c r="J23" s="85" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="L23" s="30" t="s">
         <v>36</v>
@@ -2634,7 +2701,7 @@
     </row>
     <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="68" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>9</v>
@@ -2646,7 +2713,7 @@
         <v>29</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="L24" s="31" t="s">
         <v>61</v>
@@ -2655,10 +2722,10 @@
     </row>
     <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="71" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="H25" s="23" t="s">
         <v>30</v>
@@ -2667,16 +2734,16 @@
         <v>38</v>
       </c>
       <c r="J25" s="86" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="N25" s="35"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="72" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H26" s="41" t="s">
         <v>60</v>
@@ -2685,20 +2752,20 @@
         <v>39</v>
       </c>
       <c r="J26" s="87" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L26" s="33"/>
       <c r="N26" s="35"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H27" s="82" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I27" s="40" t="s">
         <v>11</v>
@@ -2710,7 +2777,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="71" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H28" s="38" t="s">
         <v>38</v>
@@ -2749,12 +2816,12 @@
         <v>16</v>
       </c>
       <c r="J30" s="51" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B31" s="7"/>
       <c r="H31" s="37" t="s">
@@ -2767,7 +2834,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H32" s="38" t="s">
         <v>27</v>
@@ -2779,7 +2846,7 @@
     </row>
     <row r="33" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B33" s="39"/>
       <c r="D33" s="35"/>
@@ -2794,7 +2861,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B34" s="7"/>
       <c r="H34" s="38" t="s">
@@ -2807,7 +2874,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B35" s="7"/>
       <c r="H35" s="38" t="s">

</xml_diff>